<commit_message>
add timer for breath count
</commit_message>
<xml_diff>
--- a/config/default/forms/app/immunization_and_growth.xlsx
+++ b/config/default/forms/app/immunization_and_growth.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="629">
   <si>
     <t>type</t>
   </si>
@@ -1133,9 +1133,6 @@
   </si>
   <si>
     <t>The next follow up visit for ${patient_name} will be in 3 days after ${next_appointment_date}</t>
-  </si>
-  <si>
-    <t>Follow up ${patient_name} on return within 1 day</t>
   </si>
   <si>
     <t>The next follow up visit for ${patient_name} will be in  1 day after ${developmental_next_assignment_date}</t>
@@ -10966,7 +10963,7 @@
       </c>
       <c r="B188" s="48"/>
       <c r="C188" s="57" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D188" s="49"/>
       <c r="E188" s="49"/>
@@ -11012,7 +11009,7 @@
       </c>
       <c r="B189" s="48"/>
       <c r="C189" s="58" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D189" s="49"/>
       <c r="E189" s="49"/>
@@ -11596,7 +11593,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="65" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B1" s="65" t="s">
         <v>1</v>
@@ -11638,13 +11635,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="67" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
@@ -11668,13 +11665,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="67" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B3" s="67" t="s">
+        <v>369</v>
+      </c>
+      <c r="C3" s="67" t="s">
         <v>370</v>
-      </c>
-      <c r="C3" s="67" t="s">
-        <v>371</v>
       </c>
       <c r="D3" s="68"/>
       <c r="E3" s="68"/>
@@ -11722,13 +11719,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="67" t="s">
+        <v>371</v>
+      </c>
+      <c r="B5" s="67" t="s">
         <v>372</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="C5" s="67" t="s">
         <v>373</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>374</v>
       </c>
       <c r="D5" s="68"/>
       <c r="E5" s="68"/>
@@ -11752,13 +11749,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="67" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B6" s="69" t="s">
+        <v>374</v>
+      </c>
+      <c r="C6" s="69" t="s">
         <v>375</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>376</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="68"/>
@@ -11782,13 +11779,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="67" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B7" s="67" t="s">
+        <v>376</v>
+      </c>
+      <c r="C7" s="67" t="s">
         <v>377</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>378</v>
       </c>
       <c r="D7" s="68"/>
       <c r="E7" s="68"/>
@@ -11812,13 +11809,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="67" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B8" s="67" t="s">
+        <v>378</v>
+      </c>
+      <c r="C8" s="67" t="s">
         <v>379</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>380</v>
       </c>
       <c r="D8" s="68"/>
       <c r="E8" s="68"/>
@@ -11866,13 +11863,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="67" t="s">
+        <v>380</v>
+      </c>
+      <c r="B10" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="C10" s="67" t="s">
         <v>382</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>383</v>
       </c>
       <c r="D10" s="68"/>
       <c r="E10" s="68"/>
@@ -11896,13 +11893,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="67" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B11" s="69" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" s="67" t="s">
         <v>384</v>
-      </c>
-      <c r="C11" s="67" t="s">
-        <v>385</v>
       </c>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
@@ -11950,13 +11947,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="70" t="s">
+        <v>385</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="70" t="s">
         <v>387</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>388</v>
       </c>
       <c r="D13" s="68"/>
       <c r="E13" s="68"/>
@@ -11980,13 +11977,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="70" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C14" s="70" t="s">
         <v>389</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>390</v>
       </c>
       <c r="D14" s="68"/>
       <c r="E14" s="68"/>
@@ -12010,13 +12007,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="70" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C15" s="70" t="s">
         <v>391</v>
-      </c>
-      <c r="C15" s="70" t="s">
-        <v>392</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="68"/>
@@ -12064,13 +12061,13 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="70" t="s">
+        <v>392</v>
+      </c>
+      <c r="B17" s="70" t="s">
+        <v>369</v>
+      </c>
+      <c r="C17" s="70" t="s">
         <v>393</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>370</v>
-      </c>
-      <c r="C17" s="70" t="s">
-        <v>394</v>
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
@@ -12094,13 +12091,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="70" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B18" s="70" t="s">
         <v>83</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="68"/>
@@ -12148,13 +12145,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="70" t="s">
+        <v>395</v>
+      </c>
+      <c r="B20" s="68" t="s">
         <v>396</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="C20" s="70" t="s">
         <v>397</v>
-      </c>
-      <c r="C20" s="70" t="s">
-        <v>398</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
@@ -12178,13 +12175,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="70" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B21" s="68" t="s">
+        <v>398</v>
+      </c>
+      <c r="C21" s="70" t="s">
         <v>399</v>
-      </c>
-      <c r="C21" s="70" t="s">
-        <v>400</v>
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
@@ -12208,13 +12205,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="70" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B22" s="68" t="s">
+        <v>400</v>
+      </c>
+      <c r="C22" s="70" t="s">
         <v>401</v>
-      </c>
-      <c r="C22" s="70" t="s">
-        <v>402</v>
       </c>
       <c r="D22" s="68"/>
       <c r="E22" s="68"/>
@@ -12238,13 +12235,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="70" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B23" s="70" t="s">
+        <v>402</v>
+      </c>
+      <c r="C23" s="70" t="s">
         <v>403</v>
-      </c>
-      <c r="C23" s="70" t="s">
-        <v>404</v>
       </c>
       <c r="D23" s="68"/>
       <c r="E23" s="68"/>
@@ -12268,13 +12265,13 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="70" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>405</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>406</v>
       </c>
       <c r="D24" s="68"/>
       <c r="E24" s="68"/>
@@ -12320,13 +12317,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="70" t="s">
+        <v>406</v>
+      </c>
+      <c r="B26" s="71" t="s">
         <v>407</v>
       </c>
-      <c r="B26" s="71" t="s">
+      <c r="C26" s="70" t="s">
         <v>408</v>
-      </c>
-      <c r="C26" s="70" t="s">
-        <v>409</v>
       </c>
       <c r="D26" s="68"/>
       <c r="E26" s="68"/>
@@ -12350,13 +12347,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B27" s="70" t="s">
+        <v>409</v>
+      </c>
+      <c r="C27" s="70" t="s">
         <v>410</v>
-      </c>
-      <c r="C27" s="70" t="s">
-        <v>411</v>
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="68"/>
@@ -12380,13 +12377,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B28" s="70" t="s">
+        <v>411</v>
+      </c>
+      <c r="C28" s="70" t="s">
         <v>412</v>
-      </c>
-      <c r="C28" s="70" t="s">
-        <v>413</v>
       </c>
       <c r="D28" s="68"/>
       <c r="E28" s="68"/>
@@ -12410,13 +12407,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B29" s="68" t="s">
+        <v>396</v>
+      </c>
+      <c r="C29" s="71" t="s">
         <v>397</v>
-      </c>
-      <c r="C29" s="71" t="s">
-        <v>398</v>
       </c>
       <c r="D29" s="68"/>
       <c r="E29" s="68"/>
@@ -12440,13 +12437,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B30" s="68" t="s">
+        <v>398</v>
+      </c>
+      <c r="C30" s="70" t="s">
         <v>399</v>
-      </c>
-      <c r="C30" s="70" t="s">
-        <v>400</v>
       </c>
       <c r="D30" s="68"/>
       <c r="E30" s="68"/>
@@ -12470,13 +12467,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B31" s="68" t="s">
+        <v>400</v>
+      </c>
+      <c r="C31" s="70" t="s">
         <v>401</v>
-      </c>
-      <c r="C31" s="70" t="s">
-        <v>402</v>
       </c>
       <c r="D31" s="68"/>
       <c r="E31" s="68"/>
@@ -12500,13 +12497,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B32" s="70" t="s">
+        <v>402</v>
+      </c>
+      <c r="C32" s="70" t="s">
         <v>403</v>
-      </c>
-      <c r="C32" s="70" t="s">
-        <v>404</v>
       </c>
       <c r="D32" s="68"/>
       <c r="E32" s="68"/>
@@ -12530,13 +12527,13 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>405</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>406</v>
       </c>
       <c r="D33" s="68"/>
       <c r="E33" s="68"/>
@@ -12584,70 +12581,70 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>415</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>418</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B39" s="9">
         <v>3.0</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B40" s="9">
         <v>7.0</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B41" s="9">
         <v>13.0</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B42" s="9">
         <v>14.0</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -12682,13 +12679,13 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="74" t="s">
+        <v>424</v>
+      </c>
+      <c r="B45" s="74" t="s">
         <v>425</v>
       </c>
-      <c r="B45" s="74" t="s">
+      <c r="C45" s="74" t="s">
         <v>426</v>
-      </c>
-      <c r="C45" s="74" t="s">
-        <v>427</v>
       </c>
       <c r="D45" s="62"/>
       <c r="E45" s="62"/>
@@ -12715,13 +12712,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="75" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B46" s="75" t="s">
         <v>63</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D46" s="62"/>
       <c r="E46" s="62"/>
@@ -12778,7 +12775,7 @@
         <v>87</v>
       </c>
       <c r="B48" s="62" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C48" s="62" t="s">
         <v>91</v>
@@ -12811,7 +12808,7 @@
         <v>87</v>
       </c>
       <c r="B49" s="62" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C49" s="62" t="s">
         <v>99</v>
@@ -12844,10 +12841,10 @@
         <v>87</v>
       </c>
       <c r="B50" s="62" t="s">
+        <v>430</v>
+      </c>
+      <c r="C50" s="62" t="s">
         <v>431</v>
-      </c>
-      <c r="C50" s="62" t="s">
-        <v>432</v>
       </c>
       <c r="D50" s="62"/>
       <c r="E50" s="62"/>
@@ -12877,10 +12874,10 @@
         <v>87</v>
       </c>
       <c r="B51" s="62" t="s">
+        <v>432</v>
+      </c>
+      <c r="C51" s="62" t="s">
         <v>433</v>
-      </c>
-      <c r="C51" s="62" t="s">
-        <v>434</v>
       </c>
       <c r="D51" s="62"/>
       <c r="E51" s="62"/>
@@ -12910,7 +12907,7 @@
         <v>87</v>
       </c>
       <c r="B52" s="62" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C52" s="62" t="s">
         <v>122</v>
@@ -12943,7 +12940,7 @@
         <v>87</v>
       </c>
       <c r="B53" s="62" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C53" s="62" t="s">
         <v>117</v>
@@ -12976,10 +12973,10 @@
         <v>87</v>
       </c>
       <c r="B54" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C54" s="62" t="s">
         <v>437</v>
-      </c>
-      <c r="C54" s="62" t="s">
-        <v>438</v>
       </c>
       <c r="D54" s="62"/>
       <c r="E54" s="62"/>
@@ -13009,10 +13006,10 @@
         <v>87</v>
       </c>
       <c r="B55" s="62" t="s">
+        <v>438</v>
+      </c>
+      <c r="C55" s="62" t="s">
         <v>439</v>
-      </c>
-      <c r="C55" s="62" t="s">
-        <v>440</v>
       </c>
       <c r="D55" s="62"/>
       <c r="E55" s="62"/>
@@ -13042,10 +13039,10 @@
         <v>87</v>
       </c>
       <c r="B56" s="67" t="s">
+        <v>440</v>
+      </c>
+      <c r="C56" s="62" t="s">
         <v>441</v>
-      </c>
-      <c r="C56" s="62" t="s">
-        <v>442</v>
       </c>
       <c r="D56" s="62"/>
       <c r="E56" s="62"/>
@@ -13076,10 +13073,10 @@
         <v>102</v>
       </c>
       <c r="B58" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>443</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -13087,10 +13084,10 @@
         <v>102</v>
       </c>
       <c r="B59" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>445</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
@@ -13098,10 +13095,10 @@
         <v>102</v>
       </c>
       <c r="B60" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>447</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
@@ -13109,10 +13106,10 @@
         <v>102</v>
       </c>
       <c r="B61" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>449</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
@@ -13121,10 +13118,10 @@
         <v>133</v>
       </c>
       <c r="B63" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>451</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
@@ -13132,10 +13129,10 @@
         <v>133</v>
       </c>
       <c r="B64" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>453</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
@@ -13143,10 +13140,10 @@
         <v>133</v>
       </c>
       <c r="B65" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>455</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1"/>
@@ -13155,10 +13152,10 @@
         <v>125</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
@@ -13166,10 +13163,10 @@
         <v>125</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
@@ -13177,10 +13174,10 @@
         <v>125</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
@@ -13193,10 +13190,10 @@
         <v>141</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -13204,10 +13201,10 @@
         <v>141</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1"/>
@@ -13216,10 +13213,10 @@
         <v>149</v>
       </c>
       <c r="B74" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>462</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
@@ -13227,10 +13224,10 @@
         <v>149</v>
       </c>
       <c r="B75" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>464</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1"/>
@@ -13239,10 +13236,10 @@
         <v>163</v>
       </c>
       <c r="B77" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>466</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
@@ -13250,10 +13247,10 @@
         <v>163</v>
       </c>
       <c r="B78" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>468</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
@@ -13261,10 +13258,10 @@
         <v>163</v>
       </c>
       <c r="B79" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>470</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
@@ -13272,10 +13269,10 @@
         <v>163</v>
       </c>
       <c r="B80" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>472</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
@@ -13283,10 +13280,10 @@
         <v>163</v>
       </c>
       <c r="B81" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>474</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
@@ -13294,10 +13291,10 @@
         <v>163</v>
       </c>
       <c r="B82" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>476</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
@@ -13305,10 +13302,10 @@
         <v>163</v>
       </c>
       <c r="B83" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>478</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
@@ -13316,10 +13313,10 @@
         <v>163</v>
       </c>
       <c r="B84" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>480</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
@@ -13327,10 +13324,10 @@
         <v>163</v>
       </c>
       <c r="B85" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>482</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
@@ -13338,110 +13335,110 @@
         <v>163</v>
       </c>
       <c r="B86" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="C86" s="9" t="s">
         <v>484</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1"/>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B88" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="C88" s="9" t="s">
         <v>487</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B89" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>489</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
@@ -13452,10 +13449,10 @@
         <v>216</v>
       </c>
       <c r="B98" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="C98" s="9" t="s">
         <v>498</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
@@ -13463,10 +13460,10 @@
         <v>216</v>
       </c>
       <c r="B99" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="C99" s="9" t="s">
         <v>500</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
@@ -13474,10 +13471,10 @@
         <v>216</v>
       </c>
       <c r="B100" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="C100" s="9" t="s">
         <v>502</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
@@ -13501,10 +13498,10 @@
         <v>220</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
@@ -13512,10 +13509,10 @@
         <v>220</v>
       </c>
       <c r="B104" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C104" s="9" t="s">
         <v>505</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
@@ -13536,76 +13533,76 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="71" t="s">
+        <v>506</v>
+      </c>
+      <c r="B107" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="C107" s="9" t="s">
         <v>508</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="71" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B108" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="C108" s="9" t="s">
         <v>510</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="71" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B109" s="9" t="s">
+        <v>511</v>
+      </c>
+      <c r="C109" s="9" t="s">
         <v>512</v>
-      </c>
-      <c r="C109" s="9" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="71" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B110" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="C110" s="9" t="s">
         <v>514</v>
-      </c>
-      <c r="C110" s="9" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="71" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="C111" s="9" t="s">
         <v>516</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="71" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B112" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="C112" s="9" t="s">
         <v>518</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="71" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>306</v>
@@ -13618,43 +13615,43 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="71" t="s">
+        <v>520</v>
+      </c>
+      <c r="B115" s="9" t="s">
         <v>521</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="C115" s="9" t="s">
         <v>522</v>
-      </c>
-      <c r="C115" s="9" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="71" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B116" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="C116" s="9" t="s">
         <v>524</v>
-      </c>
-      <c r="C116" s="9" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="71" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B117" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="C117" s="9" t="s">
         <v>526</v>
-      </c>
-      <c r="C117" s="9" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="71" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C118" s="9" t="s">
         <v>306</v>
@@ -13667,7 +13664,7 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B120" s="71" t="s">
         <v>295</v>
@@ -13678,10 +13675,10 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="71" t="s">
+        <v>528</v>
+      </c>
+      <c r="B121" s="71" t="s">
         <v>529</v>
-      </c>
-      <c r="B121" s="71" t="s">
-        <v>530</v>
       </c>
       <c r="C121" s="9" t="s">
         <v>298</v>
@@ -13689,7 +13686,7 @@
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B122" s="71" t="s">
         <v>299</v>
@@ -13700,10 +13697,10 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B123" s="71" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C123" s="9" t="s">
         <v>302</v>
@@ -13711,7 +13708,7 @@
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B124" s="9" t="s">
         <v>303</v>
@@ -13722,7 +13719,7 @@
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>305</v>
@@ -13733,13 +13730,13 @@
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B126" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="C126" s="9" t="s">
         <v>532</v>
-      </c>
-      <c r="C126" s="9" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
@@ -13868,25 +13865,25 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="65" t="s">
+        <v>533</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>534</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="C1" s="65" t="s">
         <v>535</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="D1" s="65" t="s">
         <v>536</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="E1" s="65" t="s">
         <v>537</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="F1" s="65" t="s">
         <v>538</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="G1" s="77" t="s">
         <v>539</v>
-      </c>
-      <c r="G1" s="77" t="s">
-        <v>540</v>
       </c>
       <c r="H1" s="65"/>
       <c r="I1" s="65"/>
@@ -13910,24 +13907,24 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="78" t="s">
+        <v>540</v>
+      </c>
+      <c r="B2" s="78" t="s">
         <v>541</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>542</v>
       </c>
       <c r="C2" s="79" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-12-11_16-45</v>
+        <v>2020-12-14_12-44</v>
       </c>
       <c r="D2" s="80" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E2" s="80" t="s">
         <v>310</v>
       </c>
       <c r="F2" s="62"/>
       <c r="G2" s="81" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H2" s="62"/>
       <c r="I2" s="62"/>
@@ -14253,7 +14250,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="65" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B1" s="65" t="s">
         <v>1</v>
@@ -14296,13 +14293,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="68" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B2" s="68" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="68" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
@@ -14327,13 +14324,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="68" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B3" s="68" t="s">
+        <v>369</v>
+      </c>
+      <c r="C3" s="68" t="s">
         <v>370</v>
-      </c>
-      <c r="C3" s="68" t="s">
-        <v>371</v>
       </c>
       <c r="D3" s="68"/>
       <c r="E3" s="68"/>
@@ -14383,13 +14380,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="68" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B5" s="68" t="s">
+        <v>544</v>
+      </c>
+      <c r="C5" s="68" t="s">
         <v>545</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>546</v>
       </c>
       <c r="D5" s="68"/>
       <c r="E5" s="68"/>
@@ -14414,13 +14411,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="68" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B6" s="68" t="s">
+        <v>546</v>
+      </c>
+      <c r="C6" s="68" t="s">
         <v>547</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>548</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="68"/>
@@ -14445,13 +14442,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="68" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B7" s="68" t="s">
+        <v>548</v>
+      </c>
+      <c r="C7" s="68" t="s">
         <v>549</v>
-      </c>
-      <c r="C7" s="68" t="s">
-        <v>550</v>
       </c>
       <c r="D7" s="68"/>
       <c r="E7" s="68"/>
@@ -14476,13 +14473,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="68" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B8" s="68" t="s">
+        <v>550</v>
+      </c>
+      <c r="C8" s="68" t="s">
         <v>551</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>552</v>
       </c>
       <c r="D8" s="68"/>
       <c r="E8" s="68"/>
@@ -14507,13 +14504,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="68" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B9" s="68" t="s">
+        <v>552</v>
+      </c>
+      <c r="C9" s="68" t="s">
         <v>553</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>554</v>
       </c>
       <c r="D9" s="68"/>
       <c r="E9" s="68"/>
@@ -14563,13 +14560,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="68" t="s">
+        <v>554</v>
+      </c>
+      <c r="B11" s="68" t="s">
         <v>555</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="C11" s="68" t="s">
         <v>556</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>557</v>
       </c>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
@@ -14594,13 +14591,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="68" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B12" s="68" t="s">
+        <v>557</v>
+      </c>
+      <c r="C12" s="68" t="s">
         <v>558</v>
-      </c>
-      <c r="C12" s="68" t="s">
-        <v>559</v>
       </c>
       <c r="D12" s="68"/>
       <c r="E12" s="68"/>
@@ -14625,13 +14622,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="68" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B13" s="68" t="s">
+        <v>559</v>
+      </c>
+      <c r="C13" s="68" t="s">
         <v>560</v>
-      </c>
-      <c r="C13" s="68" t="s">
-        <v>561</v>
       </c>
       <c r="D13" s="68"/>
       <c r="E13" s="68"/>
@@ -14656,13 +14653,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="68" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B14" s="68" t="s">
+        <v>561</v>
+      </c>
+      <c r="C14" s="68" t="s">
         <v>562</v>
-      </c>
-      <c r="C14" s="68" t="s">
-        <v>563</v>
       </c>
       <c r="D14" s="68"/>
       <c r="E14" s="68"/>
@@ -14687,13 +14684,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="68" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B15" s="68" t="s">
+        <v>563</v>
+      </c>
+      <c r="C15" s="68" t="s">
         <v>564</v>
-      </c>
-      <c r="C15" s="68" t="s">
-        <v>565</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="68"/>
@@ -14718,13 +14715,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="68" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B16" s="68" t="s">
+        <v>565</v>
+      </c>
+      <c r="C16" s="68" t="s">
         <v>566</v>
-      </c>
-      <c r="C16" s="68" t="s">
-        <v>567</v>
       </c>
       <c r="D16" s="68"/>
       <c r="E16" s="68"/>
@@ -14774,13 +14771,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B18" s="68" t="s">
+        <v>555</v>
+      </c>
+      <c r="C18" s="68" t="s">
         <v>556</v>
-      </c>
-      <c r="C18" s="68" t="s">
-        <v>557</v>
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="68"/>
@@ -14805,13 +14802,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B19" s="68" t="s">
+        <v>557</v>
+      </c>
+      <c r="C19" s="68" t="s">
         <v>558</v>
-      </c>
-      <c r="C19" s="68" t="s">
-        <v>559</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="68"/>
@@ -14836,13 +14833,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B20" s="68" t="s">
+        <v>559</v>
+      </c>
+      <c r="C20" s="68" t="s">
         <v>560</v>
-      </c>
-      <c r="C20" s="68" t="s">
-        <v>561</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
@@ -14867,13 +14864,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B21" s="68" t="s">
+        <v>561</v>
+      </c>
+      <c r="C21" s="68" t="s">
         <v>562</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>563</v>
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
@@ -14898,13 +14895,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B22" s="68" t="s">
+        <v>565</v>
+      </c>
+      <c r="C22" s="68" t="s">
         <v>566</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>567</v>
       </c>
       <c r="D22" s="68"/>
       <c r="E22" s="68"/>
@@ -14929,13 +14926,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="68" t="s">
+        <v>567</v>
+      </c>
+      <c r="B23" s="68" t="s">
         <v>568</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="C23" s="68" t="s">
         <v>569</v>
-      </c>
-      <c r="C23" s="68" t="s">
-        <v>570</v>
       </c>
       <c r="D23" s="68"/>
       <c r="E23" s="68"/>
@@ -14985,13 +14982,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B25" s="68" t="s">
+        <v>396</v>
+      </c>
+      <c r="C25" s="68" t="s">
         <v>397</v>
-      </c>
-      <c r="C25" s="68" t="s">
-        <v>398</v>
       </c>
       <c r="D25" s="68"/>
       <c r="E25" s="68"/>
@@ -15016,13 +15013,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B26" s="68" t="s">
+        <v>398</v>
+      </c>
+      <c r="C26" s="68" t="s">
         <v>399</v>
-      </c>
-      <c r="C26" s="68" t="s">
-        <v>400</v>
       </c>
       <c r="D26" s="68"/>
       <c r="E26" s="68"/>
@@ -15047,13 +15044,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B27" s="68" t="s">
+        <v>400</v>
+      </c>
+      <c r="C27" s="68" t="s">
         <v>401</v>
-      </c>
-      <c r="C27" s="68" t="s">
-        <v>402</v>
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="68"/>
@@ -15078,13 +15075,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="68" t="s">
+        <v>570</v>
+      </c>
+      <c r="B28" s="68" t="s">
         <v>571</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="C28" s="68" t="s">
         <v>572</v>
-      </c>
-      <c r="C28" s="68" t="s">
-        <v>573</v>
       </c>
       <c r="D28" s="68"/>
       <c r="E28" s="68"/>
@@ -15109,10 +15106,10 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B29" s="68" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C29" s="68" t="s">
         <v>306</v>
@@ -15165,13 +15162,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="68" t="s">
+        <v>574</v>
+      </c>
+      <c r="B31" s="68" t="s">
         <v>575</v>
       </c>
-      <c r="B31" s="68" t="s">
-        <v>576</v>
-      </c>
       <c r="C31" s="68" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D31" s="68"/>
       <c r="E31" s="68"/>
@@ -15196,13 +15193,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="68" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B32" s="68" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C32" s="68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D32" s="68"/>
       <c r="E32" s="68"/>
@@ -15252,118 +15249,118 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B42" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B43" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C43" t="s">
         <v>306</v>
@@ -15377,26 +15374,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="2"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="2"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -15407,13 +15404,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="89" t="s">
+        <v>590</v>
+      </c>
+      <c r="B48" s="89" t="s">
         <v>591</v>
       </c>
-      <c r="B48" s="89" t="s">
+      <c r="C48" s="89" t="s">
         <v>592</v>
-      </c>
-      <c r="C48" s="89" t="s">
-        <v>593</v>
       </c>
       <c r="D48" s="89"/>
       <c r="E48" s="89"/>
@@ -15438,13 +15435,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="89" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B49" s="89" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C49" s="89" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D49" s="89"/>
       <c r="E49" s="89"/>
@@ -15470,65 +15467,65 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
+        <v>594</v>
+      </c>
+      <c r="B51" t="s">
         <v>595</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>596</v>
-      </c>
-      <c r="C51" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B52" t="s">
+        <v>597</v>
+      </c>
+      <c r="C52" t="s">
         <v>598</v>
-      </c>
-      <c r="C52" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B53" t="s">
+        <v>599</v>
+      </c>
+      <c r="C53" t="s">
         <v>600</v>
-      </c>
-      <c r="C53" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B54" t="s">
+        <v>601</v>
+      </c>
+      <c r="C54" t="s">
         <v>602</v>
-      </c>
-      <c r="C54" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B55" t="s">
+        <v>603</v>
+      </c>
+      <c r="C55" t="s">
         <v>604</v>
-      </c>
-      <c r="C55" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B56" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C56" t="s">
         <v>306</v>
@@ -15537,43 +15534,43 @@
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="89" t="s">
+        <v>605</v>
+      </c>
+      <c r="B58" s="89" t="s">
         <v>606</v>
       </c>
-      <c r="B58" s="89" t="s">
+      <c r="C58" s="89" t="s">
         <v>607</v>
-      </c>
-      <c r="C58" s="89" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="89" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B59" s="89" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C59" s="89" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="89" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B60" s="89" t="s">
+        <v>609</v>
+      </c>
+      <c r="C60" s="89" t="s">
         <v>610</v>
-      </c>
-      <c r="C60" s="89" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="89" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B61" s="89" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C61" s="89" t="s">
         <v>306</v>
@@ -15582,111 +15579,111 @@
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="62" t="s">
+        <v>611</v>
+      </c>
+      <c r="B63" s="62" t="s">
         <v>612</v>
       </c>
-      <c r="B63" s="62" t="s">
+      <c r="C63" s="89" t="s">
         <v>613</v>
-      </c>
-      <c r="C63" s="89" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="62" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B64" s="62" t="s">
+        <v>614</v>
+      </c>
+      <c r="C64" s="89" t="s">
         <v>615</v>
-      </c>
-      <c r="C64" s="89" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="62" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B65" s="62" t="s">
+        <v>616</v>
+      </c>
+      <c r="C65" s="89" t="s">
         <v>617</v>
-      </c>
-      <c r="C65" s="89" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="62" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B66" s="62" t="s">
+        <v>618</v>
+      </c>
+      <c r="C66" s="89" t="s">
         <v>619</v>
-      </c>
-      <c r="C66" s="89" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="62" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B67" s="62" t="s">
+        <v>404</v>
+      </c>
+      <c r="C67" s="89" t="s">
         <v>405</v>
-      </c>
-      <c r="C67" s="89" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
+        <v>620</v>
+      </c>
+      <c r="B69" t="s">
         <v>621</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>622</v>
-      </c>
-      <c r="C69" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B70" t="s">
+        <v>623</v>
+      </c>
+      <c r="C70" t="s">
         <v>624</v>
-      </c>
-      <c r="C70" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
+        <v>625</v>
+      </c>
+      <c r="B72" t="s">
         <v>626</v>
       </c>
-      <c r="B72" t="s">
-        <v>627</v>
-      </c>
       <c r="C72" s="90" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B73" t="s">
+        <v>627</v>
+      </c>
+      <c r="C73" t="s">
         <v>628</v>
-      </c>
-      <c r="C73" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B74" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C74" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
moar taskss for child assess
</commit_message>
<xml_diff>
--- a/config/default/forms/app/immunization_and_growth.xlsx
+++ b/config/default/forms/app/immunization_and_growth.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="682">
   <si>
     <t>type</t>
   </si>
@@ -752,7 +752,7 @@
     <t>growth_monitoring_vit_a</t>
   </si>
   <si>
-    <t>Did the child receive Vitamin A supplimentation?</t>
+    <t>Did the child receive Vitamin A supplement?</t>
   </si>
   <si>
     <t>${patient_age_in_months} &gt;= 5</t>
@@ -1747,10 +1747,13 @@
     <t>feeding_method_complimentary</t>
   </si>
   <si>
+    <t>Complementary feeding</t>
+  </si>
+  <si>
+    <t>feeding_method_complimentary_2</t>
+  </si>
+  <si>
     <t>Complimentary feeding</t>
-  </si>
-  <si>
-    <t>feeding_method_complimentary_2</t>
   </si>
   <si>
     <t>feeding_method_feeding</t>
@@ -14078,7 +14081,7 @@
         <v>555</v>
       </c>
       <c r="C103" s="71" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
@@ -14086,10 +14089,10 @@
         <v>244</v>
       </c>
       <c r="B104" s="71" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C104" s="71" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
@@ -14110,76 +14113,76 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="72" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B107" s="71" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C107" s="71" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="72" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B108" s="71" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C108" s="71" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="72" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B109" s="71" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C109" s="71" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="72" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B110" s="71" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C110" s="71" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="72" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B111" s="71" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C111" s="71" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="72" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B112" s="71" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C112" s="71" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="72" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B113" s="71" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C113" s="71" t="s">
         <v>329</v>
@@ -14192,43 +14195,43 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="72" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B115" s="71" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C115" s="71" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="72" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B116" s="71" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C116" s="71" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="72" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B117" s="71" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C117" s="71" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="72" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B118" s="71" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C118" s="71" t="s">
         <v>329</v>
@@ -14241,7 +14244,7 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="72" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B120" s="72" t="s">
         <v>318</v>
@@ -14252,10 +14255,10 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="72" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B121" s="72" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C121" s="71" t="s">
         <v>321</v>
@@ -14263,7 +14266,7 @@
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="72" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B122" s="72" t="s">
         <v>322</v>
@@ -14274,10 +14277,10 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="72" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B123" s="72" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C123" s="71" t="s">
         <v>325</v>
@@ -14285,7 +14288,7 @@
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="72" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B124" s="71" t="s">
         <v>326</v>
@@ -14296,7 +14299,7 @@
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="72" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B125" s="71" t="s">
         <v>328</v>
@@ -14307,13 +14310,13 @@
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="72" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B126" s="71" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C126" s="71" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
@@ -14442,25 +14445,25 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C1" s="64" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D1" s="64" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E1" s="64" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F1" s="64" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="G1" s="78" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="H1" s="64"/>
       <c r="I1" s="64"/>
@@ -14484,24 +14487,24 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="79" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C2" s="80" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2021-01-26_15-27</v>
+        <v>2021-01-28_15-38</v>
       </c>
       <c r="D2" s="81" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="E2" s="81" t="s">
         <v>417</v>
       </c>
       <c r="F2" s="66"/>
       <c r="G2" s="82" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="H2" s="66"/>
       <c r="I2" s="66"/>
@@ -14960,10 +14963,10 @@
         <v>432</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C5" s="68" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D5" s="68"/>
       <c r="E5" s="68"/>
@@ -14991,10 +14994,10 @@
         <v>432</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C6" s="68" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="68"/>
@@ -15022,10 +15025,10 @@
         <v>432</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C7" s="68" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D7" s="68"/>
       <c r="E7" s="68"/>
@@ -15053,10 +15056,10 @@
         <v>432</v>
       </c>
       <c r="B8" s="68" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C8" s="68" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D8" s="68"/>
       <c r="E8" s="68"/>
@@ -15084,10 +15087,10 @@
         <v>432</v>
       </c>
       <c r="B9" s="68" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D9" s="68"/>
       <c r="E9" s="68"/>
@@ -15137,13 +15140,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="68" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B11" s="68" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C11" s="68" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
@@ -15168,13 +15171,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="68" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C12" s="68" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D12" s="68"/>
       <c r="E12" s="68"/>
@@ -15199,13 +15202,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="68" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C13" s="68" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D13" s="68"/>
       <c r="E13" s="68"/>
@@ -15230,13 +15233,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="68" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C14" s="68" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D14" s="68"/>
       <c r="E14" s="68"/>
@@ -15261,13 +15264,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="68" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B15" s="68" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C15" s="68" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="68"/>
@@ -15292,13 +15295,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="68" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C16" s="68" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D16" s="68"/>
       <c r="E16" s="68"/>
@@ -15348,13 +15351,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="68" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C18" s="68" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="68"/>
@@ -15379,13 +15382,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="68" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C19" s="68" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="68"/>
@@ -15410,13 +15413,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="68" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C20" s="68" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
@@ -15441,13 +15444,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="68" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C21" s="68" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
@@ -15472,13 +15475,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="68" t="s">
+        <v>620</v>
+      </c>
+      <c r="B22" s="68" t="s">
+        <v>618</v>
+      </c>
+      <c r="C22" s="68" t="s">
         <v>619</v>
-      </c>
-      <c r="B22" s="68" t="s">
-        <v>617</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>618</v>
       </c>
       <c r="D22" s="68"/>
       <c r="E22" s="68"/>
@@ -15503,13 +15506,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="68" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C23" s="68" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D23" s="68"/>
       <c r="E23" s="68"/>
@@ -15559,7 +15562,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="68" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B25" s="68" t="s">
         <v>448</v>
@@ -15590,7 +15593,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="68" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B26" s="68" t="s">
         <v>450</v>
@@ -15621,7 +15624,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="68" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B27" s="68" t="s">
         <v>452</v>
@@ -15652,13 +15655,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="68" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B28" s="68" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C28" s="68" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D28" s="68"/>
       <c r="E28" s="68"/>
@@ -15683,10 +15686,10 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="68" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B29" s="68" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C29" s="68" t="s">
         <v>329</v>
@@ -15739,10 +15742,10 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="68" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B31" s="68" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C31" s="68" t="s">
         <v>420</v>
@@ -15770,10 +15773,10 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="68" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B32" s="68" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C32" s="68" t="s">
         <v>422</v>
@@ -15826,118 +15829,118 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B42" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B43" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C43" t="s">
         <v>329</v>
@@ -15951,26 +15954,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="2"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="2"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -15981,13 +15984,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="90" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B48" s="90" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C48" s="90" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D48" s="90"/>
       <c r="E48" s="90"/>
@@ -16012,10 +16015,10 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="90" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B49" s="90" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C49" s="90" t="s">
         <v>479</v>
@@ -16044,65 +16047,65 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B51" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C51" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B52" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C52" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B53" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C53" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B54" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C54" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B55" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C55" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B56" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C56" t="s">
         <v>329</v>
@@ -16111,43 +16114,43 @@
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="90" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B58" s="90" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C58" s="90" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="90" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B59" s="90" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C59" s="90" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="90" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B60" s="90" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C60" s="90" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="90" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B61" s="90" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C61" s="90" t="s">
         <v>329</v>
@@ -16156,51 +16159,51 @@
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="66" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B63" s="66" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C63" s="90" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="66" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B64" s="66" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C64" s="90" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="66" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B65" s="66" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C65" s="90" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="66" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B66" s="66" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C66" s="90" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="66" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B67" s="66" t="s">
         <v>456</v>
@@ -16212,55 +16215,55 @@
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B69" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C69" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B70" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C70" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B72" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C72" s="91" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B73" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C73" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B74" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C74" t="s">
         <v>329</v>

</xml_diff>